<commit_message>
Re-ran MATLAB code with behavioral n36, added session number to behavioral clock, added design file for behavioral follow-up, moved csv read-in into getSubjInfo.m
</commit_message>
<xml_diff>
--- a/analysis/clock_questionnaires_n36.xlsx
+++ b/analysis/clock_questionnaires_n36.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="163">
   <si>
     <t>ASWS:</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Returning to Wakefulness</t>
   </si>
   <si>
-    <t>SCORE</t>
-  </si>
-  <si>
     <t>TAS</t>
   </si>
   <si>
@@ -127,9 +124,6 @@
     <t>CD</t>
   </si>
   <si>
-    <t>NonAccept</t>
-  </si>
-  <si>
     <t>custom data</t>
   </si>
   <si>
@@ -506,6 +500,15 @@
   </si>
   <si>
     <t>UPPS_Prem</t>
+  </si>
+  <si>
+    <t>RPI</t>
+  </si>
+  <si>
+    <t>DERS_NonAccept</t>
+  </si>
+  <si>
+    <t>RSE</t>
   </si>
 </sst>
 </file>
@@ -513,8 +516,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="179" formatCode="mm/dd/yy;@"/>
-    <numFmt numFmtId="185" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -820,12 +823,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -834,10 +837,10 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="185" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="179" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -872,8 +875,8 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="185" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="179" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -882,7 +885,7 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1328,9 +1331,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CA44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="CB2" sqref="CB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1354,7 +1357,7 @@
       <c r="D1" s="26"/>
       <c r="E1" s="24"/>
       <c r="F1" s="24" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G1" s="13" t="s">
         <v>0</v>
@@ -1425,7 +1428,7 @@
         <v>9</v>
       </c>
       <c r="BC1" s="31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="BD1" s="31"/>
       <c r="BE1" s="31"/>
@@ -1438,7 +1441,7 @@
       <c r="BL1" s="31"/>
       <c r="BM1" s="30"/>
       <c r="BN1" s="33" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="BO1" s="33"/>
       <c r="BP1" s="33"/>
@@ -1446,12 +1449,12 @@
       <c r="BR1" s="33"/>
       <c r="BS1" s="33"/>
       <c r="BT1" s="34" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="BU1" s="34"/>
       <c r="BV1" s="34"/>
       <c r="BW1" s="35" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="BX1" s="35"/>
       <c r="BY1" s="35"/>
@@ -1460,22 +1463,22 @@
     </row>
     <row r="2" spans="1:79" s="11" customFormat="1" ht="52.5" customHeight="1">
       <c r="A2" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>39</v>
-      </c>
       <c r="F2" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>10</v>
@@ -1493,208 +1496,208 @@
         <v>14</v>
       </c>
       <c r="L2" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="S2" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="U2" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="V2" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="W2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="X2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z2" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="M2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="S2" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="T2" s="10" t="s">
+      <c r="AA2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="AK2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM2" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="AN2" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="AO2" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="U2" s="10" t="s">
+      <c r="AP2" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="V2" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="W2" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="X2" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y2" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z2" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="AA2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC2" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD2" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE2" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF2" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH2" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI2" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ2" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="AK2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL2" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="AM2" s="9" t="s">
+      <c r="AQ2" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="AR2" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="AS2" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="AT2" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="AN2" s="9" t="s">
+      <c r="AU2" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="AO2" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="AP2" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="AQ2" s="9" t="s">
+      <c r="AV2" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="AR2" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="AS2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="AT2" s="9" t="s">
+      <c r="AW2" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="AX2" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="AY2" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="AZ2" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="AU2" s="9" t="s">
+      <c r="BA2" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="AV2" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="AW2" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="AX2" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="AY2" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="AZ2" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="BA2" s="9" t="s">
-        <v>150</v>
-      </c>
       <c r="BB2" s="9" t="s">
-        <v>15</v>
+        <v>162</v>
       </c>
       <c r="BC2" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="BD2" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="BE2" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="BD2" s="12" t="s">
+      <c r="BF2" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="BE2" s="12" t="s">
+      <c r="BG2" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="BF2" s="12" t="s">
+      <c r="BH2" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="BG2" s="12" t="s">
+      <c r="BI2" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="BH2" s="12" t="s">
+      <c r="BJ2" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="BI2" s="12" t="s">
+      <c r="BK2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="BJ2" s="12" t="s">
+      <c r="BL2" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="BK2" s="12" t="s">
+      <c r="BM2" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="BL2" s="12" t="s">
+      <c r="BN2" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="BM2" s="12" t="s">
+      <c r="BO2" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="BN2" s="12" t="s">
+      <c r="BP2" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="BO2" s="12" t="s">
+      <c r="BQ2" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="BP2" s="11" t="s">
+      <c r="BR2" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="BQ2" s="11" t="s">
+      <c r="BS2" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="BR2" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="BS2" s="11" t="s">
-        <v>69</v>
-      </c>
       <c r="BT2" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="BU2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="BV2" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="BW2" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="BU2" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="BV2" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="BW2" s="11" t="s">
+      <c r="BX2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="BY2" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="BX2" s="11" t="s">
+      <c r="BZ2" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="BY2" s="11" t="s">
+      <c r="CA2" s="11" t="s">
         <v>50</v>
-      </c>
-      <c r="BZ2" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="CA2" s="11" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:79" s="2" customFormat="1">
@@ -1711,7 +1714,7 @@
         <v>41360</v>
       </c>
       <c r="E3" s="25">
-        <f>ROUND(((D3-C3)/365.25),2)</f>
+        <f t="shared" ref="E3:E38" si="0">ROUND(((D3-C3)/365.25),2)</f>
         <v>20.9</v>
       </c>
       <c r="F3" s="25">
@@ -1901,7 +1904,7 @@
         <v>2</v>
       </c>
       <c r="BP3" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BQ3" s="2">
         <v>2</v>
@@ -1919,7 +1922,7 @@
         <v>13</v>
       </c>
       <c r="BV3" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BW3" s="32">
         <v>57</v>
@@ -1951,7 +1954,7 @@
         <v>41353</v>
       </c>
       <c r="E4" s="57">
-        <f>ROUND(((D4-C4)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>18.18</v>
       </c>
       <c r="F4" s="57">
@@ -2144,13 +2147,13 @@
         <v>3</v>
       </c>
       <c r="BQ4" s="58" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BR4" s="58" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BS4" s="58" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BT4" s="58">
         <v>10</v>
@@ -2189,7 +2192,7 @@
         <v>41373</v>
       </c>
       <c r="E5" s="40">
-        <f>ROUND(((D5-C5)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>16.309999999999999</v>
       </c>
       <c r="F5" s="40">
@@ -2382,13 +2385,13 @@
         <v>3</v>
       </c>
       <c r="BQ5" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BR5" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BS5" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BT5" s="41">
         <v>13</v>
@@ -2429,7 +2432,7 @@
         <v>41389</v>
       </c>
       <c r="E6" s="25">
-        <f>ROUND(((D6-C6)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>21.75</v>
       </c>
       <c r="F6" s="25">
@@ -2619,7 +2622,7 @@
         <v>1</v>
       </c>
       <c r="BP6" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BQ6" s="2">
         <v>3</v>
@@ -2637,7 +2640,7 @@
         <v>12</v>
       </c>
       <c r="BV6" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BW6" s="32">
         <v>52</v>
@@ -2669,7 +2672,7 @@
         <v>41407</v>
       </c>
       <c r="E7" s="25">
-        <f>ROUND(((D7-C7)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>22.41</v>
       </c>
       <c r="F7" s="25">
@@ -2859,7 +2862,7 @@
         <v>5</v>
       </c>
       <c r="BP7" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BQ7" s="2">
         <v>2</v>
@@ -2877,7 +2880,7 @@
         <v>10</v>
       </c>
       <c r="BV7" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BW7" s="32">
         <v>61</v>
@@ -2909,7 +2912,7 @@
         <v>41404</v>
       </c>
       <c r="E8" s="40">
-        <f>ROUND(((D8-C8)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>15.39</v>
       </c>
       <c r="F8" s="40">
@@ -3102,13 +3105,13 @@
         <v>7</v>
       </c>
       <c r="BQ8" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BR8" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BS8" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BT8" s="41">
         <v>10</v>
@@ -3147,7 +3150,7 @@
         <v>41380</v>
       </c>
       <c r="E9" s="40">
-        <f>ROUND(((D9-C9)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>15.44</v>
       </c>
       <c r="F9" s="40">
@@ -3340,13 +3343,13 @@
         <v>4</v>
       </c>
       <c r="BQ9" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BR9" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BS9" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BT9" s="41">
         <v>11</v>
@@ -3355,7 +3358,7 @@
         <v>12</v>
       </c>
       <c r="BV9" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BW9" s="43">
         <v>57</v>
@@ -3387,7 +3390,7 @@
         <v>41403</v>
       </c>
       <c r="E10" s="40">
-        <f>ROUND(((D10-C10)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>16.78</v>
       </c>
       <c r="F10" s="40">
@@ -3580,13 +3583,13 @@
         <v>4</v>
       </c>
       <c r="BQ10" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BR10" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BS10" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BT10" s="41">
         <v>11</v>
@@ -3595,7 +3598,7 @@
         <v>11</v>
       </c>
       <c r="BV10" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BW10" s="43">
         <v>47</v>
@@ -3627,7 +3630,7 @@
         <v>41361</v>
       </c>
       <c r="E11" s="40">
-        <f>ROUND(((D11-C11)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>15.53</v>
       </c>
       <c r="F11" s="40">
@@ -3820,13 +3823,13 @@
         <v>7</v>
       </c>
       <c r="BQ11" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BR11" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BS11" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BT11" s="41">
         <v>13</v>
@@ -3867,7 +3870,7 @@
         <v>41400</v>
       </c>
       <c r="E12" s="40">
-        <f>ROUND(((D12-C12)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>15.87</v>
       </c>
       <c r="F12" s="40">
@@ -4060,13 +4063,13 @@
         <v>4</v>
       </c>
       <c r="BQ12" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BR12" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BS12" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BT12" s="41">
         <v>9</v>
@@ -4107,7 +4110,7 @@
         <v>41353</v>
       </c>
       <c r="E13" s="25">
-        <f>ROUND(((D13-C13)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>19.84</v>
       </c>
       <c r="F13" s="25">
@@ -4297,7 +4300,7 @@
         <v>2</v>
       </c>
       <c r="BP13" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BQ13" s="2">
         <v>2</v>
@@ -4315,7 +4318,7 @@
         <v>14</v>
       </c>
       <c r="BV13" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BW13" s="32">
         <v>48</v>
@@ -4347,7 +4350,7 @@
         <v>41332</v>
       </c>
       <c r="E14" s="25">
-        <f>ROUND(((D14-C14)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>22.85</v>
       </c>
       <c r="F14" s="25">
@@ -4537,7 +4540,7 @@
         <v>2</v>
       </c>
       <c r="BP14" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BQ14" s="2">
         <v>5</v>
@@ -4587,7 +4590,7 @@
         <v>41386</v>
       </c>
       <c r="E15" s="40">
-        <f>ROUND(((D15-C15)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>14.65</v>
       </c>
       <c r="F15" s="40">
@@ -4780,13 +4783,13 @@
         <v>5</v>
       </c>
       <c r="BQ15" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BR15" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BS15" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BT15" s="41">
         <v>9</v>
@@ -4827,7 +4830,7 @@
         <v>41366</v>
       </c>
       <c r="E16" s="25">
-        <f>ROUND(((D16-C16)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>19.11</v>
       </c>
       <c r="F16" s="25">
@@ -5017,7 +5020,7 @@
         <v>2</v>
       </c>
       <c r="BP16" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BQ16" s="2">
         <v>2</v>
@@ -5035,7 +5038,7 @@
         <v>10</v>
       </c>
       <c r="BV16" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BW16" s="32">
         <v>54</v>
@@ -5067,7 +5070,7 @@
         <v>41388</v>
       </c>
       <c r="E17" s="40">
-        <f>ROUND(((D17-C17)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>14.43</v>
       </c>
       <c r="F17" s="40">
@@ -5260,13 +5263,13 @@
         <v>3</v>
       </c>
       <c r="BQ17" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BR17" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BS17" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BT17" s="41">
         <v>12</v>
@@ -5307,7 +5310,7 @@
         <v>41387</v>
       </c>
       <c r="E18" s="40">
-        <f>ROUND(((D18-C18)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>14.73</v>
       </c>
       <c r="F18" s="40">
@@ -5500,13 +5503,13 @@
         <v>2</v>
       </c>
       <c r="BQ18" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BR18" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BS18" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BT18" s="41">
         <v>11</v>
@@ -5515,7 +5518,7 @@
         <v>11</v>
       </c>
       <c r="BV18" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BW18" s="43">
         <v>57</v>
@@ -5547,7 +5550,7 @@
         <v>41379</v>
       </c>
       <c r="E19" s="25">
-        <f>ROUND(((D19-C19)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>21.88</v>
       </c>
       <c r="F19" s="25">
@@ -5737,7 +5740,7 @@
         <v>4</v>
       </c>
       <c r="BP19" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BQ19" s="2">
         <v>3</v>
@@ -5787,7 +5790,7 @@
         <v>41383</v>
       </c>
       <c r="E20" s="40">
-        <f>ROUND(((D20-C20)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>15.07</v>
       </c>
       <c r="F20" s="40">
@@ -5980,13 +5983,13 @@
         <v>2</v>
       </c>
       <c r="BQ20" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BR20" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BS20" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BT20" s="41">
         <v>9</v>
@@ -6027,7 +6030,7 @@
         <v>41396</v>
       </c>
       <c r="E21" s="25">
-        <f>ROUND(((D21-C21)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>21.35</v>
       </c>
       <c r="F21" s="25">
@@ -6133,25 +6136,25 @@
         <v>150</v>
       </c>
       <c r="AN21" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AO21" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AP21" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AQ21" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AR21" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AS21" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AT21" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AU21" s="2">
         <v>27</v>
@@ -6217,7 +6220,7 @@
         <v>3</v>
       </c>
       <c r="BP21" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BQ21" s="2">
         <v>2</v>
@@ -6235,7 +6238,7 @@
         <v>12</v>
       </c>
       <c r="BV21" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BW21" s="32">
         <v>52</v>
@@ -6258,7 +6261,7 @@
         <v>10152</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C22" s="61">
         <v>34099</v>
@@ -6267,7 +6270,7 @@
         <v>41411</v>
       </c>
       <c r="E22" s="25">
-        <f>ROUND(((D22-C22)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>20.02</v>
       </c>
       <c r="F22" s="25">
@@ -6451,7 +6454,7 @@
         <v>0</v>
       </c>
       <c r="BP22" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BT22" s="2">
         <v>11</v>
@@ -6463,19 +6466,19 @@
         <v>12</v>
       </c>
       <c r="BW22" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BX22" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BY22" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BZ22" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="CA22" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:79" s="2" customFormat="1">
@@ -6492,7 +6495,7 @@
         <v>41416</v>
       </c>
       <c r="E23" s="25">
-        <f>ROUND(((D23-C23)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>23.79</v>
       </c>
       <c r="F23" s="2">
@@ -6686,7 +6689,7 @@
         <v>4</v>
       </c>
       <c r="BP23" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BQ23" s="2">
         <v>4</v>
@@ -6698,13 +6701,13 @@
         <v>3</v>
       </c>
       <c r="BT23" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BU23" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BV23" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BW23" s="63">
         <v>64</v>
@@ -6736,7 +6739,7 @@
         <v>41417</v>
       </c>
       <c r="E24" s="25">
-        <f>ROUND(((D24-C24)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>29.28</v>
       </c>
       <c r="F24" s="25">
@@ -6930,7 +6933,7 @@
         <v>6</v>
       </c>
       <c r="BP24" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BQ24" s="2">
         <v>2</v>
@@ -6942,13 +6945,13 @@
         <v>5</v>
       </c>
       <c r="BT24" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BU24" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BV24" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BW24" s="63">
         <v>59</v>
@@ -6980,7 +6983,7 @@
         <v>41423</v>
       </c>
       <c r="E25" s="25">
-        <f>ROUND(((D25-C25)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>30.84</v>
       </c>
       <c r="F25" s="2">
@@ -7168,7 +7171,7 @@
         <v>9</v>
       </c>
       <c r="BP25" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BQ25" s="2">
         <v>4</v>
@@ -7218,7 +7221,7 @@
         <v>41429</v>
       </c>
       <c r="E26" s="25">
-        <f>ROUND(((D26-C26)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>24.13</v>
       </c>
       <c r="F26" s="25">
@@ -7412,7 +7415,7 @@
         <v>2</v>
       </c>
       <c r="BP26" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BQ26" s="2">
         <v>2</v>
@@ -7430,7 +7433,7 @@
         <v>12</v>
       </c>
       <c r="BV26" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BW26" s="63">
         <v>64</v>
@@ -7462,7 +7465,7 @@
         <v>41428</v>
       </c>
       <c r="E27" s="25">
-        <f>ROUND(((D27-C27)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>27.46</v>
       </c>
       <c r="F27" s="25">
@@ -7656,7 +7659,7 @@
         <v>5</v>
       </c>
       <c r="BP27" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BQ27" s="2">
         <v>4</v>
@@ -7674,7 +7677,7 @@
         <v>12</v>
       </c>
       <c r="BV27" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BW27" s="63">
         <v>67</v>
@@ -7697,7 +7700,7 @@
         <v>11184</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C28" s="61">
         <v>32321</v>
@@ -7706,7 +7709,7 @@
         <v>41446</v>
       </c>
       <c r="E28" s="25">
-        <f>ROUND(((D28-C28)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>24.98</v>
       </c>
       <c r="F28" s="2">
@@ -7857,79 +7860,79 @@
         <v>18</v>
       </c>
       <c r="BC28" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BD28" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BE28" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BF28" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BG28" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BH28" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BI28" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BJ28" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BK28" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BL28" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BM28" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BN28" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BO28" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BP28" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BQ28" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BR28" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BS28" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BT28" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BU28" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BV28" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BW28" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BX28" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BY28" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BZ28" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="CA28" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:79" s="2" customFormat="1">
@@ -7946,7 +7949,7 @@
         <v>41464</v>
       </c>
       <c r="E29" s="25">
-        <f>ROUND(((D29-C29)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>26.67</v>
       </c>
       <c r="F29" s="25">
@@ -8136,7 +8139,7 @@
         <v>4</v>
       </c>
       <c r="BP29" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BQ29" s="2">
         <v>4</v>
@@ -8186,7 +8189,7 @@
         <v>41452</v>
       </c>
       <c r="E30" s="25">
-        <f>ROUND(((D30-C30)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>27.95</v>
       </c>
       <c r="F30" s="25">
@@ -8376,7 +8379,7 @@
         <v>3</v>
       </c>
       <c r="BP30" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BQ30" s="2">
         <v>3</v>
@@ -8426,7 +8429,7 @@
         <v>41464</v>
       </c>
       <c r="E31" s="25">
-        <f>ROUND(((D31-C31)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>28.82</v>
       </c>
       <c r="F31" s="25">
@@ -8613,7 +8616,7 @@
         <v>3</v>
       </c>
       <c r="BP31" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BQ31" s="2">
         <v>7</v>
@@ -8663,7 +8666,7 @@
         <v>41436</v>
       </c>
       <c r="E32" s="25">
-        <f>ROUND(((D32-C32)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>31.01</v>
       </c>
       <c r="F32" s="25">
@@ -8853,7 +8856,7 @@
         <v>5</v>
       </c>
       <c r="BP32" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BQ32" s="2">
         <v>3</v>
@@ -8903,7 +8906,7 @@
         <v>41453</v>
       </c>
       <c r="E33" s="25">
-        <f>ROUND(((D33-C33)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>30.76</v>
       </c>
       <c r="F33" s="25">
@@ -9093,7 +9096,7 @@
         <v>6</v>
       </c>
       <c r="BP33" s="70" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BQ33" s="70">
         <v>6</v>
@@ -9111,7 +9114,7 @@
         <v>14</v>
       </c>
       <c r="BV33" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BW33" s="63">
         <v>53</v>
@@ -9143,7 +9146,7 @@
         <v>41478</v>
       </c>
       <c r="E34" s="25">
-        <f>ROUND(((D34-C34)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>25.98</v>
       </c>
       <c r="F34" s="2">
@@ -9333,7 +9336,7 @@
         <v>8</v>
       </c>
       <c r="BP34" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BQ34" s="2">
         <v>8</v>
@@ -9351,7 +9354,7 @@
         <v>15</v>
       </c>
       <c r="BV34" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BW34" s="2">
         <v>51</v>
@@ -9383,7 +9386,7 @@
         <v>41478</v>
       </c>
       <c r="E35" s="25">
-        <f>ROUND(((D35-C35)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>26.84</v>
       </c>
       <c r="F35" s="25">
@@ -9577,7 +9580,7 @@
         <v>2</v>
       </c>
       <c r="BP35" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BQ35" s="2">
         <v>5</v>
@@ -9618,7 +9621,7 @@
         <v>10385</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C36" s="61">
         <v>32293</v>
@@ -9627,7 +9630,7 @@
         <v>41484</v>
       </c>
       <c r="E36" s="25">
-        <f>ROUND(((D36-C36)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>25.16</v>
       </c>
       <c r="F36" s="2">
@@ -9778,55 +9781,55 @@
         <v>18</v>
       </c>
       <c r="BC36" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BD36" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BE36" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BF36" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BG36" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BH36" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BI36" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BJ36" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BK36" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BL36" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BM36" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BN36" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BO36" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BP36" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BQ36" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BR36" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BS36" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BT36" s="2">
         <v>3</v>
@@ -9838,19 +9841,19 @@
         <v>13</v>
       </c>
       <c r="BW36" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BX36" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BY36" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BZ36" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="CA36" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:79" s="2" customFormat="1">
@@ -9867,7 +9870,7 @@
         <v>41484</v>
       </c>
       <c r="E37" s="25">
-        <f>ROUND(((D37-C37)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>27.31</v>
       </c>
       <c r="F37" s="2">
@@ -10057,7 +10060,7 @@
         <v>2</v>
       </c>
       <c r="BP37" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BQ37" s="2">
         <v>5</v>
@@ -10107,7 +10110,7 @@
         <v>41492</v>
       </c>
       <c r="E38" s="25">
-        <f>ROUND(((D38-C38)/365.25),2)</f>
+        <f t="shared" si="0"/>
         <v>23.58</v>
       </c>
       <c r="F38" s="2">
@@ -10299,7 +10302,7 @@
         <v>3</v>
       </c>
       <c r="BP38" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BQ38" s="2">
         <v>2</v>
@@ -10412,205 +10415,205 @@
   <sheetData>
     <row r="1" spans="1:68" ht="36.75" customHeight="1">
       <c r="A1" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="G1" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="H1" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="I1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="K1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="BO1" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:68">

</xml_diff>